<commit_message>
updated boost converter, eliminated unnecessary tuning components, rotated oscillator, updated solar pads
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="28740" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BOM" localSheetId="0">Sheet1!$A$5:$J$40</definedName>
+    <definedName name="BOM" localSheetId="0">Sheet1!$A$5:$J$38</definedName>
   </definedNames>
   <calcPr calcId="140000" iterate="1" concurrentCalc="0"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="222">
   <si>
     <t>Qty</t>
   </si>
@@ -61,12 +61,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>RESISTOR0603-RES</t>
-  </si>
-  <si>
-    <t>0603-RES</t>
-  </si>
-  <si>
     <t>Resistor</t>
   </si>
   <si>
@@ -166,18 +160,12 @@
     <t>C22, C23</t>
   </si>
   <si>
-    <t>47uH</t>
-  </si>
-  <si>
     <t>INDUCTOR0603</t>
   </si>
   <si>
     <t>L4</t>
   </si>
   <si>
-    <t>L2</t>
-  </si>
-  <si>
     <t>6.8 uH</t>
   </si>
   <si>
@@ -268,15 +256,6 @@
     <t>U$2</t>
   </si>
   <si>
-    <t>MM5329-2700</t>
-  </si>
-  <si>
-    <t>MM5829-2700</t>
-  </si>
-  <si>
-    <t>U$3, U$7</t>
-  </si>
-  <si>
     <t>PANASONIC_RECTIFIER</t>
   </si>
   <si>
@@ -301,18 +280,9 @@
     <t>Venus838FLPx-L</t>
   </si>
   <si>
-    <t>311-0.0GRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0603JR-070RL</t>
-  </si>
-  <si>
     <t>Yageo</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/yageo/RC0603JR-070RL/311-0.0GRCT-ND/729622</t>
-  </si>
-  <si>
     <t>C1, C2, C3, C4, C5, C7, C9, C14, C15, C17, C18</t>
   </si>
   <si>
@@ -400,9 +370,6 @@
     <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERA-2AED103X/P10KDECT-ND/1706304</t>
   </si>
   <si>
-    <t>R6, R7, R8, R9, R12,R18</t>
-  </si>
-  <si>
     <t>490-5924-2-ND</t>
   </si>
   <si>
@@ -463,27 +430,9 @@
     <t>Inductor</t>
   </si>
   <si>
-    <t>445-3610-6-ND</t>
-  </si>
-  <si>
-    <t>GLFR1608T470M-LR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/tdk-corporation/GLFR1608T470M-LR/445-3610-6-ND/1856777</t>
-  </si>
-  <si>
-    <t>712-1431-2-ND</t>
-  </si>
-  <si>
-    <t>L-14C5N6SV4T</t>
-  </si>
-  <si>
     <t>Johanson Technology</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/johanson-technology-inc/L-14C5N6SV4T/712-1431-2-ND/1561298</t>
-  </si>
-  <si>
     <t>445-1023-2-ND</t>
   </si>
   <si>
@@ -614,27 +563,6 @@
   </si>
   <si>
     <t>Boost Converter</t>
-  </si>
-  <si>
-    <t>497-6106-1-ND</t>
-  </si>
-  <si>
-    <t>L6920DCTR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/stmicroelectronics/L6920DCTR/497-6106-1-ND/1654032</t>
-  </si>
-  <si>
-    <t>Coaxial Connector</t>
-  </si>
-  <si>
-    <t>90-5894-1-ND</t>
-  </si>
-  <si>
-    <t>MM5829-2700RJ4</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/MM5829-2700RJ4/490-5894-1-ND/3528184</t>
   </si>
   <si>
     <t>Full bridge rectifier</t>
@@ -723,9 +651,6 @@
     <t>I will mail these to you</t>
   </si>
   <si>
-    <t>0 nH</t>
-  </si>
-  <si>
     <t>2.2nH</t>
   </si>
   <si>
@@ -741,9 +666,6 @@
     <t>https://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=251947178&amp;uq=636552498736187867</t>
   </si>
   <si>
-    <t>R13, R15, R21, R22</t>
-  </si>
-  <si>
     <t>CAP0603-CAP</t>
   </si>
   <si>
@@ -762,9 +684,6 @@
     <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM1885C1H101JA01D/490-1427-1-ND/587633</t>
   </si>
   <si>
-    <t>R14, R16, R17</t>
-  </si>
-  <si>
     <t>712-1621-1-ND</t>
   </si>
   <si>
@@ -778,13 +697,43 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/molex-llc/0467650301/WM11254CT-ND/5287246</t>
+  </si>
+  <si>
+    <t>497-3368-1-ND</t>
+  </si>
+  <si>
+    <t>L6920DTR</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stmicroelectronics/L6920DTR/497-3368-1-ND/668269</t>
+  </si>
+  <si>
+    <t>R6, R7, R8, R9, R12</t>
+  </si>
+  <si>
+    <t>10uH</t>
+  </si>
+  <si>
+    <t>ASPI-0315FS</t>
+  </si>
+  <si>
+    <t>535-10735-2-ND</t>
+  </si>
+  <si>
+    <t>ASPI-0315FS-100M-T2</t>
+  </si>
+  <si>
+    <t>Abracon LLC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.in/product-detail/en/abracon-llc/ASPI-0315FS-100M-T2/535-10735-2-ND/2619300</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -811,14 +760,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -878,32 +819,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -917,19 +858,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="13" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="14" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="18">
     <cellStyle name="Bad" xfId="1" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -940,9 +879,11 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Good" xfId="14" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="13" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1276,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1291,147 +1232,147 @@
     <col min="5" max="5" width="23.1640625" customWidth="1"/>
     <col min="6" max="6" width="42" customWidth="1"/>
     <col min="7" max="7" width="51.5" customWidth="1"/>
-    <col min="8" max="8" width="21" style="9" customWidth="1"/>
+    <col min="8" max="8" width="21" style="8" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
     <col min="10" max="10" width="29.83203125" customWidth="1"/>
     <col min="11" max="11" width="19.1640625" customWidth="1"/>
     <col min="12" max="12" width="112.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1">
-      <c r="A1" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="H1" s="8"/>
+    <row r="1" spans="1:12" s="5" customFormat="1">
+      <c r="A1" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="A2" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
+      <c r="A3" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>189</v>
+      <c r="H5" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="13">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
+      <c r="A6" s="10">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>226</v>
+        <v>80</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>87</v>
+        <v>193</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>89</v>
+        <v>79</v>
+      </c>
+      <c r="L6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="13">
+      <c r="A7" s="10">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="13">
+      <c r="A8" s="10">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1439,35 +1380,35 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="L8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="13">
+      <c r="A9" s="10">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1475,35 +1416,35 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="13">
+      <c r="A10" s="10">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1511,71 +1452,71 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="L10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="13">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="9" customFormat="1">
+      <c r="A11" s="10">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>106</v>
+        <v>204</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>107</v>
+        <v>205</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="10" customFormat="1">
-      <c r="A12" s="13">
+        <v>94</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="10">
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1583,755 +1524,755 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>228</v>
+        <v>20</v>
+      </c>
+      <c r="E12" s="1">
+        <v>805</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>229</v>
+        <v>21</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>230</v>
+        <v>99</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>231</v>
+        <v>100</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>232</v>
+        <v>90</v>
+      </c>
+      <c r="L12" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="13">
+      <c r="A13" s="10">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="1">
-        <v>805</v>
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="L13" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="13">
-        <v>1</v>
+      <c r="A14" s="10">
+        <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="10">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="13">
-        <v>6</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="L15" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="13">
-        <v>2</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>29</v>
+      <c r="A16" s="10">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1">
+        <v>180</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>104</v>
       </c>
       <c r="L16" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="13">
-        <v>3</v>
-      </c>
-      <c r="B17" s="1">
-        <v>180</v>
+      <c r="A17" s="10">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="L17" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="13">
-        <v>1</v>
+      <c r="A18" s="10">
+        <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="L18" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="13">
-        <v>2</v>
+      <c r="A19" s="10">
+        <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="L19" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="13">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>36</v>
+      <c r="A20" s="10">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>330</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="10">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L20" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="13">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1">
-        <v>330</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="E21" s="1">
+        <v>805</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>136</v>
+        <v>182</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L21" t="s">
-        <v>138</v>
+        <v>94</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="13">
-        <v>2</v>
+      <c r="A22" s="10">
+        <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>216</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="1">
-        <v>805</v>
+        <v>217</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="13">
+        <v>220</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="1" customFormat="1">
+      <c r="A23" s="10">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>196</v>
+      </c>
       <c r="D23" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E23" s="1">
         <v>603</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>197</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>141</v>
+        <v>193</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="1" customFormat="1">
-      <c r="A24" s="13">
+        <v>129</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="10">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>221</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E24" s="1">
         <v>603</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>222</v>
+        <v>42</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>224</v>
+        <v>193</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>225</v>
+        <v>86</v>
+      </c>
+      <c r="L24" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="13">
-        <v>1</v>
+      <c r="A25" s="10">
+        <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="1">
-        <v>603</v>
+        <v>45</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>46</v>
+        <v>169</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="L25" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="13">
-        <v>2</v>
+      <c r="A26" s="10">
+        <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="H26" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="10">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="L26" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="13">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="1">
+        <v>32.768000000000001</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="10">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="L27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="13">
-        <v>1</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" s="1">
-        <v>32.768000000000001</v>
-      </c>
       <c r="G28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="J28" s="3">
+        <v>467650301</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="10">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="L28" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="13">
-        <v>1</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="10">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="J29" s="4">
-        <v>467650301</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="L29" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="13">
-        <v>1</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="10">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="L30" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="13">
-        <v>1</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="10">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="L31" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="13">
-        <v>1</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="H32" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>191</v>
+        <v>153</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>192</v>
+        <v>154</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>193</v>
+        <v>155</v>
+      </c>
+      <c r="L32" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="13">
-        <v>2</v>
+      <c r="A33" s="10">
+        <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>65</v>
@@ -2350,23 +2291,23 @@
         <v>68</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="L33" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="13">
+      <c r="A34" s="10">
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2377,354 +2318,208 @@
         <v>69</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="L34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="10">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="L34" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="13">
-        <v>1</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="10">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="L35" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="13">
-        <v>2</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L36" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="10">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="13">
-        <v>1</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="13">
+      <c r="A38" s="10">
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>150</v>
+        <v>78</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>184</v>
+        <v>195</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="L38" t="s">
-        <v>185</v>
+        <v>195</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="13">
-        <v>1</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="13">
-        <v>1</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="7">
-        <v>5</v>
-      </c>
-      <c r="B41" s="7">
-        <v>0</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="K41" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="L41" s="7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="7">
+      <c r="A39" s="6">
         <v>2</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="K42" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="L42" s="7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="11">
-        <v>1</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E43" s="11">
-        <v>603</v>
-      </c>
-      <c r="F43" s="11" t="s">
+      <c r="B39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G43" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="I43" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="J43" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="K43" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="L43" s="12" t="s">
-        <v>146</v>
+      <c r="G39" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RFQ for BSU, changed matching circuit
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Sprite_CC1310_Development" localSheetId="0">Sheet1!$A$6:$I$49</definedName>
+    <definedName name="Sprite_CC1310_Development" localSheetId="0">Sheet1!$A$6:$I$48</definedName>
   </definedNames>
   <calcPr calcId="140000" iterate="1" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="Sprite_CC1310_Development.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:hunteradams:Documents:eagle:CC1310:Eagle:Sprite_CC1310_Development.txt" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:hunteradams:Documents:eagle:CC1310:Eagle:Sprite_CC1310_Development.txt" space="1" consecutive="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="289">
   <si>
     <t>Qty</t>
   </si>
@@ -154,15 +154,6 @@
     <t>R1</t>
   </si>
   <si>
-    <t>CAP0603-CAP</t>
-  </si>
-  <si>
-    <t>0603-CAP</t>
-  </si>
-  <si>
-    <t>C19</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -193,15 +184,9 @@
     <t>R11</t>
   </si>
   <si>
-    <t>2.2nH</t>
-  </si>
-  <si>
     <t>INDUCTOR0603</t>
   </si>
   <si>
-    <t>L3</t>
-  </si>
-  <si>
     <t>Inductors</t>
   </si>
   <si>
@@ -259,9 +244,6 @@
     <t>DNP</t>
   </si>
   <si>
-    <t>R17,R18,R24,R25</t>
-  </si>
-  <si>
     <t>FC-135</t>
   </si>
   <si>
@@ -496,15 +478,6 @@
     <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERA-2AEB104X/P100KDCTR-ND/1706053</t>
   </si>
   <si>
-    <t>490-1427-1-ND</t>
-  </si>
-  <si>
-    <t>GRM1885C1H101JA01D</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM1885C1H101JA01D/490-1427-1-ND/587633</t>
-  </si>
-  <si>
     <t>P10KDECT-ND</t>
   </si>
   <si>
@@ -553,18 +526,9 @@
     <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERA-2AED102X/P1.0KDECT-ND/1706280</t>
   </si>
   <si>
-    <t>712-1427-1-ND</t>
-  </si>
-  <si>
-    <t>L-14C2N2SV4T</t>
-  </si>
-  <si>
     <t>Johanson Technology</t>
   </si>
   <si>
-    <t>https://www.digikey.com/products/en?keywords=712-1427-1-ND</t>
-  </si>
-  <si>
     <t>Samsung</t>
   </si>
   <si>
@@ -725,9 +689,6 @@
   </si>
   <si>
     <t>https://www.digikey.com/products/en?keywords=LV8417CS-TE-L-HOSCT-ND</t>
-  </si>
-  <si>
-    <t>90-5894-1-ND</t>
   </si>
   <si>
     <t>MM5829-2700RJ4</t>
@@ -947,7 +908,28 @@
     <t>BOM:</t>
   </si>
   <si>
-    <t>See comments_and_instructions.txt in the provided documents</t>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>712-1431-1-ND</t>
+  </si>
+  <si>
+    <t>L-14C5N6SV4T</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/johanson-technology-inc/L-14C5N6SV4T/712-1431-1-ND/1914881</t>
+  </si>
+  <si>
+    <t>5.6nH</t>
+  </si>
+  <si>
+    <t>R17,R18,R24,R25,R27</t>
+  </si>
+  <si>
+    <t>490-5894-1-ND</t>
+  </si>
+  <si>
+    <t>See RFQ</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1034,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1128,8 +1110,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1153,8 +1140,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="80">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1226,6 +1214,11 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
@@ -1562,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1586,24 +1579,24 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="12" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="12" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="11" t="s">
-        <v>291</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="A3" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="7" spans="1:12" s="3" customFormat="1">
       <c r="A7" s="2" t="s">
@@ -1613,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>2</v>
@@ -1628,19 +1621,19 @@
         <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1664,19 +1657,19 @@
         <v>17</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1694,25 +1687,25 @@
         <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1736,19 +1729,19 @@
         <v>21</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>131</v>
-      </c>
       <c r="K10" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L10" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1772,19 +1765,19 @@
         <v>21</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L11" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1808,19 +1801,19 @@
         <v>21</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="L12" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1844,19 +1837,19 @@
         <v>21</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L13" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1880,19 +1873,19 @@
         <v>21</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L14" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1916,127 +1909,127 @@
         <v>17</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="L15" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="L16" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>149</v>
       </c>
       <c r="L17" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="11" customFormat="1">
       <c r="A18" s="1">
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>285</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="E18" s="1">
+        <v>603</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>44</v>
+        <v>281</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>160</v>
+        <v>282</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>157</v>
+        <v>283</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="L18" t="s">
-        <v>159</v>
+        <v>161</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -2044,7 +2037,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
@@ -2054,25 +2047,25 @@
         <v>20</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="L19" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -2090,25 +2083,25 @@
         <v>35</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="L20" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -2116,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
@@ -2126,105 +2119,105 @@
         <v>35</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="L21" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="1">
-        <v>603</v>
+        <v>19</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>120</v>
+        <v>21</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>171</v>
+        <v>119</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
+      </c>
+      <c r="L22" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>175</v>
+        <v>119</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="L23" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="1">
-        <v>3</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
+      </c>
+      <c r="B24" s="1">
+        <v>330</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
@@ -2234,97 +2227,97 @@
         <v>35</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>179</v>
+        <v>119</v>
+      </c>
+      <c r="I24" t="s">
+        <v>169</v>
+      </c>
+      <c r="J24" t="s">
+        <v>170</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="L24" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1">
-        <v>4</v>
-      </c>
-      <c r="B25" s="1">
-        <v>330</v>
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="E25" s="1">
+        <v>805</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I25" t="s">
-        <v>181</v>
-      </c>
-      <c r="J25" t="s">
-        <v>182</v>
+        <v>119</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="L25" t="s">
-        <v>183</v>
+        <v>133</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E26" s="1">
-        <v>805</v>
+        <v>603</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>186</v>
+        <v>123</v>
+      </c>
+      <c r="L26" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -2336,31 +2329,31 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="1">
-        <v>603</v>
+        <v>61</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>62</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>53</v>
+        <v>236</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>129</v>
+        <v>181</v>
       </c>
       <c r="L27" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -2368,35 +2361,35 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>192</v>
+        <v>119</v>
+      </c>
+      <c r="I28" t="s">
+        <v>185</v>
+      </c>
+      <c r="J28" t="s">
+        <v>183</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="L28" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -2404,35 +2397,35 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
+      </c>
+      <c r="F29" s="1">
+        <v>32.768000000000001</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I29" t="s">
-        <v>197</v>
-      </c>
-      <c r="J29" t="s">
-        <v>195</v>
+        <v>119</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="L29" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2440,35 +2433,35 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F30" s="1">
-        <v>32.768000000000001</v>
+        <v>59</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>262</v>
+        <v>60</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="L30" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2476,35 +2469,35 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>190</v>
+        <v>70</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>65</v>
+        <v>238</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="L31" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2512,35 +2505,35 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="L32" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2548,107 +2541,107 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="L33" t="s">
-        <v>212</v>
+        <v>203</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>216</v>
+        <v>207</v>
+      </c>
+      <c r="L34" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="L35" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2656,107 +2649,107 @@
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="K36" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="L36" t="s">
         <v>215</v>
-      </c>
-      <c r="L36" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>224</v>
+        <v>287</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="L37" t="s">
-        <v>227</v>
+        <v>133</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>229</v>
+        <v>119</v>
+      </c>
+      <c r="I38" t="s">
+        <v>221</v>
+      </c>
+      <c r="J38" t="s">
+        <v>220</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>230</v>
+        <v>219</v>
+      </c>
+      <c r="L38" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2764,35 +2757,35 @@
         <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I39" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="J39" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="L39" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2800,35 +2793,35 @@
         <v>1</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I40" t="s">
-        <v>235</v>
-      </c>
-      <c r="J40" t="s">
-        <v>236</v>
+        <v>119</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>226</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="L40" t="s">
-        <v>237</v>
+        <v>143</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2836,35 +2829,35 @@
         <v>1</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>267</v>
+        <v>60</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>240</v>
+        <v>193</v>
+      </c>
+      <c r="L41" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2872,32 +2865,32 @@
         <v>1</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>65</v>
+        <v>247</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>242</v>
+        <v>119</v>
+      </c>
+      <c r="I42" t="s">
+        <v>246</v>
+      </c>
+      <c r="J42" t="s">
+        <v>245</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="L42" t="s">
         <v>243</v>
@@ -2905,74 +2898,74 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G43" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I43" t="s">
         <v>260</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I43" t="s">
-        <v>259</v>
-      </c>
       <c r="J43" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="L43" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I44" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="J44" t="s">
-        <v>274</v>
+        <v>99</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>275</v>
+        <v>203</v>
       </c>
       <c r="L44" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2980,35 +2973,35 @@
         <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I45" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="J45" t="s">
-        <v>105</v>
+        <v>268</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>215</v>
+        <v>127</v>
       </c>
       <c r="L45" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -3016,137 +3009,137 @@
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>270</v>
+        <v>248</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I46" t="s">
-        <v>280</v>
-      </c>
-      <c r="J46" t="s">
-        <v>281</v>
+        <v>119</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>232</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="L46" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="1">
+        <v>187</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="3" customFormat="1">
+      <c r="A47" s="2">
         <v>1</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="K47" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="3" customFormat="1">
-      <c r="A48" s="2">
+      <c r="B47" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="J47" s="10"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="1">
         <v>1</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="I48" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="J48" s="10"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
+      <c r="B48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="1">
         <v>1</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>248</v>
+        <v>119</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>248</v>
+        <v>274</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>248</v>
+        <v>276</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -3154,104 +3147,64 @@
         <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G50" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K50" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="H50" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>285</v>
-      </c>
       <c r="L50" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="1">
-        <v>1</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="L51" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="8">
+        <v>4</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="8" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="A53" s="8">
-        <v>4</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G53" s="8" t="s">
+      <c r="G52" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="9"/>
-      <c r="L53" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
updated JTAG and UART pinouts
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="223">
   <si>
     <t>Qty</t>
   </si>
@@ -202,12 +202,6 @@
     <t>GREEN</t>
   </si>
   <si>
-    <t>HDMID</t>
-  </si>
-  <si>
-    <t>U$1</t>
-  </si>
-  <si>
     <t>JOHANSON_BALUN</t>
   </si>
   <si>
@@ -481,12 +475,6 @@
     <t>https://www.digikey.com/product-detail/en/epson/FC-135-32.7680KA-AC0/SER4084CT-ND/6132704</t>
   </si>
   <si>
-    <t>HDMI-D Female</t>
-  </si>
-  <si>
-    <t>Molex</t>
-  </si>
-  <si>
     <t>915 MHz Balun</t>
   </si>
   <si>
@@ -599,9 +587,6 @@
   </si>
   <si>
     <t>Do Not Install</t>
-  </si>
-  <si>
-    <t>DNI</t>
   </si>
   <si>
     <t>Solar Cells</t>
@@ -693,12 +678,6 @@
     <t>https://www.digikey.com/product-detail/en/johanson-technology-inc/0850BM14E0016T/712-1621-1-ND/6187665</t>
   </si>
   <si>
-    <t>WM11254CT-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/molex-llc/0467650301/WM11254CT-ND/5287246</t>
-  </si>
-  <si>
     <t>497-3368-1-ND</t>
   </si>
   <si>
@@ -727,6 +706,30 @@
   </si>
   <si>
     <t>https://www.digikey.in/product-detail/en/abracon-llc/ASPI-0315FS-100M-T2/535-10735-2-ND/2619300</t>
+  </si>
+  <si>
+    <t>CORTEX_DEBUG_SMD</t>
+  </si>
+  <si>
+    <t>SAMTECH_FTSH-105-01</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>JTAG Interface</t>
+  </si>
+  <si>
+    <t>SAM13160CT-ND</t>
+  </si>
+  <si>
+    <t>FTSH-105-01-F-DV-K-TR</t>
+  </si>
+  <si>
+    <t>Samtek Inc</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samtec-inc/FTSH-105-01-F-DV-K-TR/SAM13160CT-ND/8827915</t>
   </si>
 </sst>
 </file>
@@ -852,15 +855,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="13" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1219,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1232,7 +1233,7 @@
     <col min="5" max="5" width="23.1640625" customWidth="1"/>
     <col min="6" max="6" width="42" customWidth="1"/>
     <col min="7" max="7" width="51.5" customWidth="1"/>
-    <col min="8" max="8" width="21" style="8" customWidth="1"/>
+    <col min="8" max="8" width="21" style="7" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
     <col min="10" max="10" width="29.83203125" customWidth="1"/>
     <col min="11" max="11" width="19.1640625" customWidth="1"/>
@@ -1241,22 +1242,22 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1">
       <c r="A1" s="13" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
-      <c r="H1" s="7"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -1269,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>2</v>
@@ -1284,23 +1285,23 @@
         <v>5</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1314,29 +1315,29 @@
         <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" t="s">
         <v>81</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L6" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1356,23 +1357,23 @@
         <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="L7" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L7" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1392,23 +1393,23 @@
         <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="L8" t="s">
         <v>89</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L8" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1428,23 +1429,23 @@
         <v>10</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="L9" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L9" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1464,23 +1465,23 @@
         <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L10" t="s">
         <v>96</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="9" customFormat="1">
-      <c r="A11" s="10">
+    </row>
+    <row r="11" spans="1:12" s="8" customFormat="1">
+      <c r="A11" s="9">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1488,35 +1489,35 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>206</v>
+        <v>92</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1536,23 +1537,23 @@
         <v>10</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L12" t="s">
         <v>99</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L12" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1572,23 +1573,23 @@
         <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="L13" t="s">
         <v>103</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L13" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1602,29 +1603,29 @@
         <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L14" t="s">
         <v>106</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L14" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1644,23 +1645,23 @@
         <v>10</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" t="s">
         <v>109</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L15" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>3</v>
       </c>
       <c r="B16" s="1">
@@ -1680,23 +1681,23 @@
         <v>6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L16" t="s">
         <v>112</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L16" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="10">
+      <c r="A17" s="9">
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1716,23 +1717,23 @@
         <v>6</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I17" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L17" t="s">
         <v>115</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L17" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="10">
+      <c r="A18" s="9">
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1752,23 +1753,23 @@
         <v>10</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="L18" t="s">
         <v>119</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="L18" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="10">
+      <c r="A19" s="9">
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1788,23 +1789,23 @@
         <v>6</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L19" t="s">
         <v>122</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L19" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <v>1</v>
       </c>
       <c r="B20" s="1">
@@ -1824,23 +1825,23 @@
         <v>6</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I20" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L20" t="s">
         <v>125</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L20" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1860,63 +1861,63 @@
         <v>10</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="10">
+      <c r="A22" s="9">
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="L22" s="12" t="s">
-        <v>221</v>
+        <v>213</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="1" customFormat="1">
-      <c r="A23" s="10">
+      <c r="A23" s="9">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>39</v>
@@ -1925,29 +1926,29 @@
         <v>603</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>198</v>
-      </c>
       <c r="J23" s="3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1964,26 +1965,26 @@
         <v>42</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L24" t="s">
         <v>130</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L24" t="s">
-        <v>132</v>
-      </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -1997,29 +1998,29 @@
         <v>46</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="I25" s="2" t="s">
+      <c r="K25" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="L25" t="s">
         <v>135</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="L25" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2039,23 +2040,23 @@
         <v>49</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I26" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="L26" t="s">
         <v>139</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="L26" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="10">
+      <c r="A27" s="9">
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2075,23 +2076,23 @@
         <v>51</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="L27" t="s">
         <v>143</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="L27" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="10">
+      <c r="A28" s="9">
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2108,26 +2109,26 @@
         <v>54</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="J28" s="3">
-        <v>467650301</v>
+        <v>202</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="L28" s="11" t="s">
-        <v>211</v>
+        <v>127</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="10">
+      <c r="A29" s="9">
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2144,26 +2145,26 @@
         <v>56</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L29" t="s">
         <v>148</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="L29" s="11" t="s">
-        <v>209</v>
-      </c>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="10">
+      <c r="A30" s="9">
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2180,27 +2181,27 @@
         <v>58</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>151</v>
+        <v>206</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="L30" t="s">
-        <v>152</v>
+        <v>155</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="10">
-        <v>1</v>
+      <c r="A31" s="9">
+        <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>59</v>
@@ -2210,52 +2211,52 @@
         <v>59</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>173</v>
+        <v>62</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>212</v>
+        <v>149</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>213</v>
+        <v>150</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>214</v>
+        <v>151</v>
+      </c>
+      <c r="L31" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="10">
-        <v>2</v>
+      <c r="A32" s="9">
+        <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>153</v>
@@ -2271,43 +2272,43 @@
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="10">
+      <c r="A33" s="9">
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="L33" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="10">
+      <c r="A34" s="9">
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2324,26 +2325,26 @@
         <v>70</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="L34" t="s">
-        <v>165</v>
+        <v>102</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="10">
+      <c r="A35" s="9">
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2351,35 +2352,35 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>174</v>
+        <v>131</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>177</v>
+        <v>134</v>
+      </c>
+      <c r="L35" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="10">
+      <c r="A36" s="9">
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2387,139 +2388,137 @@
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="L36" t="s">
-        <v>168</v>
+        <v>142</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="10">
+      <c r="A37" s="9">
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>215</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>75</v>
+        <v>215</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>75</v>
+        <v>216</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>75</v>
+        <v>217</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>178</v>
+        <v>218</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>180</v>
+        <v>188</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>220</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>181</v>
+        <v>221</v>
+      </c>
+      <c r="L37" s="12" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="10">
+      <c r="A38" s="9">
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="H38" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="6">
+      <c r="A39" s="9">
         <v>2</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="D39" s="6" t="s">
+      <c r="C39" s="12"/>
+      <c r="D39" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E39" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G39" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="K39" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="L39" s="6" t="s">
-        <v>188</v>
+      <c r="G39" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="L39" s="12" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>